<commit_message>
changes to natinoal bls excel sheet
</commit_message>
<xml_diff>
--- a/Data/national_M2018_BLS.xlsx
+++ b/Data/national_M2018_BLS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thewillisgroup-my.sharepoint.com/personal/isoto_talentpath_com/Documents/H1B_and_Technology/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{19E5B7C7-6054-43AC-9172-F4D64D25A911}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EB23A556-C16B-4720-ADF3-C32682B4B468}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{19E5B7C7-6054-43AC-9172-F4D64D25A911}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{38D1EACF-F3FA-4F49-8E47-6C8AE4A300FE}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="490" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -406,7 +406,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -584,6 +584,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -747,7 +753,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -761,6 +767,9 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1144,7 +1153,7 @@
   <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:T1048576"/>
+      <selection activeCell="A3" sqref="A3:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1274,7 +1283,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1330,7 +1339,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1386,7 +1395,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1442,7 +1451,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1498,7 +1507,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1554,7 +1563,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1610,7 +1619,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1666,7 +1675,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1722,7 +1731,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1778,7 +1787,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1834,7 +1843,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1890,7 +1899,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1946,7 +1955,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -2002,7 +2011,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -2058,7 +2067,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="6" t="s">
         <v>51</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -2114,7 +2123,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="6" t="s">
         <v>53</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -2170,7 +2179,7 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="6" t="s">
         <v>55</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -2226,7 +2235,7 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="6" t="s">
         <v>57</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2282,7 +2291,7 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="6" t="s">
         <v>59</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -2338,7 +2347,7 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="6" t="s">
         <v>61</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -3233,18 +3242,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3267,18 +3276,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3FD3975-85DF-49AC-805D-8270859F84AB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD6FF11A-68DE-46D5-B607-7EC98C6C1F00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3FD3975-85DF-49AC-805D-8270859F84AB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>